<commit_message>
working on the windows laptop
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Validated Addresses" sheetId="1" r:id="rId1"/>
+    <sheet name="Validated_Results" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -375,13 +375,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>address</v>
+      </c>
+      <c r="B1" t="str">
+        <v>validatedAddresses</v>
+      </c>
+      <c r="C1" t="str">
+        <v>coordinates</v>
+      </c>
+      <c r="D1" t="str">
+        <v>resolutionQuality</v>
+      </c>
+      <c r="E1" t="str">
+        <v>taxAuthorities</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="D2" t="str">
+        <v>Intersection</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="str">
+        <v>Intersection</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>